<commit_message>
0.1.3 followers would be brought to new level now
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
   <si>
     <t>class</t>
   </si>
@@ -118,13 +118,16 @@
     <t>skeleton knight</t>
   </si>
   <si>
-    <t>0/10</t>
+    <t>0/12</t>
   </si>
   <si>
     <t>4-12</t>
   </si>
   <si>
     <t>0-6</t>
+  </si>
+  <si>
+    <t>humanity</t>
   </si>
   <si>
     <t>guard</t>
@@ -1081,7 +1084,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1237,7 +1240,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1261,23 +1264,26 @@
       </c>
       <c r="I8" t="s">
         <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>6</v>
@@ -1289,7 +1295,7 @@
         <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.2.0 statuary added, related room assigned
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46">
   <si>
     <t>class</t>
   </si>
@@ -46,6 +46,9 @@
     <t>loot</t>
   </si>
   <si>
+    <t>resist</t>
+  </si>
+  <si>
     <t>comment</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t>5/10</t>
   </si>
   <si>
+    <t>+all</t>
+  </si>
+  <si>
     <t>rat</t>
   </si>
   <si>
@@ -112,6 +118,9 @@
     <t>0.2 weapon</t>
   </si>
   <si>
+    <t>-fire</t>
+  </si>
+  <si>
     <t>burst</t>
   </si>
   <si>
@@ -128,6 +137,9 @@
   </si>
   <si>
     <t>humanity</t>
+  </si>
+  <si>
+    <t>counter &amp; combo</t>
   </si>
   <si>
     <t>guard</t>
@@ -147,9 +159,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -162,17 +174,116 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -185,80 +296,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
@@ -266,40 +310,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,91 +326,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,91 +500,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,9 +537,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,8 +564,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,7 +589,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,32 +617,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -613,145 +625,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1081,10 +1093,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1094,10 +1106,11 @@
     <col min="4" max="4" width="9" style="1"/>
     <col min="8" max="8" width="13.625" customWidth="1"/>
     <col min="10" max="10" width="15.625" customWidth="1"/>
-    <col min="11" max="11" width="21.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1"/>
+    <col min="12" max="12" width="21.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,14 +1143,17 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1146,29 +1162,32 @@
         <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -1176,13 +1195,13 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -1191,38 +1210,38 @@
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -1231,30 +1250,33 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -1263,27 +1285,33 @@
         <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F9">
         <v>6</v>
@@ -1292,10 +1320,10 @@
         <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.2.0 guide scene worked, defend bug fixed
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
   <si>
     <t>class</t>
   </si>
@@ -152,6 +152,51 @@
   </si>
   <si>
     <t>potion, armor</t>
+  </si>
+  <si>
+    <t>swarm</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>potion</t>
+  </si>
+  <si>
+    <t>split, mental</t>
+  </si>
+  <si>
+    <t>bat</t>
+  </si>
+  <si>
+    <t>15/16</t>
+  </si>
+  <si>
+    <t>5-18</t>
+  </si>
+  <si>
+    <t>0-4</t>
+  </si>
+  <si>
+    <t>+shadow</t>
+  </si>
+  <si>
+    <t>vampir | mental</t>
+  </si>
+  <si>
+    <t>crab</t>
+  </si>
+  <si>
+    <t>5/12</t>
+  </si>
+  <si>
+    <t>1-8</t>
+  </si>
+  <si>
+    <t>meat</t>
+  </si>
+  <si>
+    <t>speed=2</t>
   </si>
 </sst>
 </file>
@@ -159,9 +204,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -173,6 +218,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -181,29 +248,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,36 +290,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -255,25 +301,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,13 +325,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -302,9 +332,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,31 +371,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,151 +545,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,27 +565,34 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -571,6 +623,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -584,39 +662,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -628,7 +673,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -637,133 +682,133 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1093,10 +1138,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1326,6 +1371,96 @@
         <v>45</v>
       </c>
     </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
0.4.0 bug fix & data modified.
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
   <si>
     <t>NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,331 +134,343 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PotionOfHealing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spinner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MysteryMeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DM300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapeOfThorns</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elemental</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PotionOfLiquidFlame</t>
+  </si>
+  <si>
+    <t>Monk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Food</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>King</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>King.Undead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Succubus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScrollOfLullaby</t>
+  </si>
+  <si>
+    <t>Eye</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dewdrop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scorpio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PotionOfHealing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yog.RottingFist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yog.BurningFist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yog.Larva</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>elementalResistance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thief</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MasterThievesArmband</t>
+  </si>
+  <si>
+    <t>Properties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FetidRat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MINIBOSS DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GnollTrickster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MINIBOSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RotHeart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMMOVABLE MINIBOSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Warlock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW:0.2 HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atkSkill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defSkill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAGICAL</t>
+  </si>
+  <si>
+    <t>LIGHT:-0.2 ICE:0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.2 HOLY:-0.25 SHADOW:0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.2 HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIRE:-0.3 HOLY:-0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNDEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNDEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIRE:-0.25 SHADOW:0.25 HOLY:-0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW:0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICE:-0.15 POISON:0.3 LIGHT:-0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS MACHINE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIRE:0.5 HOLY:-0.2 ICE:-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MACHINE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MACHINE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS UNDEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNDEAD PHANTOM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW:0.2 HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.2 SHADOW:0.2 HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS DEMONIC IMMOVABLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.2 HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.2 SHADOW:0.2 HOLY:-0.25 ICE:-0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.2 HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW:0.2 POISON:0.15 FIRE:0.15 HOLY:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIGHT:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIGHT:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GreatCrab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MINIBOSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIRE:-0.25 POISON:0.2 HOLY:-0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NewbornElemental</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEMONIC MINIBOSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIGHT:0.25 POISON:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW:0.2 HOLY:-0.25 POISON:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Bat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PotionOfHealing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brute</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spinner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MysteryMeat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DM300</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapeOfThorns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Elemental</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PotionOfLiquidFlame</t>
-  </si>
-  <si>
-    <t>Monk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Food</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>King</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>King.Undead</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Succubus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScrollOfLullaby</t>
-  </si>
-  <si>
-    <t>Eye</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dewdrop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scorpio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PotionOfHealing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yog.RottingFist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yog.BurningFist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yog.Larva</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>elementalResistance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thief</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MasterThievesArmband</t>
-  </si>
-  <si>
-    <t>Properties</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FetidRat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MINIBOSS DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GnollTrickster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MINIBOSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RotHeart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IMMOVABLE MINIBOSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Warlock</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>atkSkill</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>defSkill</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MAGICAL</t>
-  </si>
-  <si>
-    <t>LIGHT:-0.2 ICE:0.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 HOLY:-0.25 SHADOW:0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIRE:-0.3 HOLY:-0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNDEAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIGHT:0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNDEAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIRE:-0.25 SHADOW:0.25 HOLY:-0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICE:-0.15 POISON:0.3 LIGHT:-0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS MACHINE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIRE:0.5 HOLY:-0.2 ICE:-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MACHINE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MACHINE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS UNDEAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNDEAD PHANTOM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 SHADOW:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS DEMONIC IMMOVABLE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 SHADOW:0.2 HOLY:-0.25 ICE:-0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2 POISON:0.15 FIRE:0.15 HOLY:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIGHT:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIGHT:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GreatCrab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MINIBOSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIRE:-0.25 POISON:0.2 HOLY:-0.3</t>
+    <t>SHADOW:0.2 FIRE:-0.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.2 ICE:-0.25</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -798,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -817,8 +829,8 @@
     <col min="12" max="12" width="10.875" customWidth="1"/>
     <col min="13" max="13" width="10.75" customWidth="1"/>
     <col min="14" max="14" width="18.125" customWidth="1"/>
-    <col min="15" max="15" width="24.125" customWidth="1"/>
-    <col min="16" max="16" width="18.125" customWidth="1"/>
+    <col min="15" max="15" width="26.375" customWidth="1"/>
+    <col min="16" max="16" width="24.75" customWidth="1"/>
     <col min="17" max="17" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -830,10 +842,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -866,10 +878,10 @@
         <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.15">
@@ -927,7 +939,7 @@
         <v>0.3</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -980,12 +992,12 @@
         <v>3</v>
       </c>
       <c r="O4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -1015,15 +1027,15 @@
         <v>2</v>
       </c>
       <c r="O5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -1056,12 +1068,12 @@
         <v>2</v>
       </c>
       <c r="P6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B7">
         <v>25</v>
@@ -1094,10 +1106,10 @@
         <v>4</v>
       </c>
       <c r="O7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
@@ -1129,10 +1141,10 @@
         <v>0.25</v>
       </c>
       <c r="O8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="P8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.15">
@@ -1196,15 +1208,15 @@
         <v>2</v>
       </c>
       <c r="O10" t="s">
+        <v>73</v>
+      </c>
+      <c r="P10" t="s">
         <v>74</v>
-      </c>
-      <c r="P10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -1225,7 +1237,7 @@
         <v>0.01</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1240,10 +1252,10 @@
         <v>3</v>
       </c>
       <c r="O11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
@@ -1275,7 +1287,7 @@
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1287,7 +1299,7 @@
         <v>0.15</v>
       </c>
       <c r="O12" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
@@ -1325,15 +1337,15 @@
         <v>6</v>
       </c>
       <c r="O13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>80</v>
@@ -1351,33 +1363,37 @@
         <v>5</v>
       </c>
       <c r="O14" t="s">
+        <v>62</v>
+      </c>
+      <c r="P14" t="s">
         <v>63</v>
       </c>
-      <c r="P14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="B15">
-        <v>150</v>
+        <v>65</v>
       </c>
       <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
         <v>20</v>
       </c>
-      <c r="D15">
-        <v>15</v>
-      </c>
-      <c r="E15">
-        <v>20</v>
-      </c>
+      <c r="H15" s="1"/>
       <c r="I15">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J15">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1386,39 +1402,30 @@
         <v>5</v>
       </c>
       <c r="N15">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="O15" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="P15" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="C16">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E16">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>16</v>
-      </c>
-      <c r="G16">
-        <v>0.1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I16">
         <v>6</v>
@@ -1427,168 +1434,177 @@
         <v>18</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N16">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="O16" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="P16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C17">
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
         <v>16</v>
       </c>
-      <c r="D17">
-        <v>15</v>
-      </c>
-      <c r="E17">
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <v>15</v>
-      </c>
       <c r="G17">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J17">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N17">
+        <v>-0.25</v>
       </c>
       <c r="O17" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="P17" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="B18">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C18">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>15</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18">
         <v>15</v>
       </c>
       <c r="G18">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="H18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I18">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J18">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B19">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>20</v>
       </c>
       <c r="D19">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19">
-        <v>0.125</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>33</v>
+        <v>0.2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>29</v>
       </c>
       <c r="I19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J19">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C20">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D20">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E20">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>16</v>
       </c>
       <c r="G20">
-        <v>0.33329999999999999</v>
+        <v>0.125</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I20">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J20">
         <v>25</v>
@@ -1597,247 +1613,250 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>10</v>
-      </c>
-      <c r="N20">
-        <v>0.25</v>
+        <v>6</v>
       </c>
       <c r="O20" t="s">
-        <v>86</v>
-      </c>
-      <c r="P20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21">
-        <v>65</v>
+        <v>200</v>
       </c>
       <c r="C21">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21">
         <v>25</v>
       </c>
-      <c r="D21">
-        <v>20</v>
-      </c>
-      <c r="E21">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>10</v>
       </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-      <c r="G21">
-        <v>0.1</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21">
-        <v>16</v>
-      </c>
-      <c r="J21">
-        <v>26</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>5</v>
-      </c>
       <c r="N21">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="O21" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="P21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B22">
         <v>65</v>
       </c>
       <c r="C22">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E22">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F22">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G22">
-        <v>0.3</v>
+        <v>0.1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="I22">
         <v>16</v>
       </c>
       <c r="J22">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="N22">
+        <v>0.2</v>
       </c>
       <c r="O22" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="P22" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
         <v>65</v>
       </c>
-      <c r="B23">
-        <v>70</v>
-      </c>
       <c r="C23">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>18</v>
       </c>
       <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="G23">
+        <v>0.3</v>
+      </c>
+      <c r="I23">
+        <v>16</v>
+      </c>
+      <c r="J23">
+        <v>30</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
         <v>10</v>
       </c>
-      <c r="F23">
-        <v>21</v>
-      </c>
-      <c r="G23">
-        <v>0.75</v>
-      </c>
-      <c r="I23">
-        <v>12</v>
-      </c>
-      <c r="J23">
-        <v>18</v>
-      </c>
-      <c r="K23" t="s">
-        <v>69</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23">
-        <v>8</v>
-      </c>
-      <c r="N23">
-        <v>0.15</v>
-      </c>
       <c r="O23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+        <v>102</v>
+      </c>
+      <c r="P23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B24">
         <v>70</v>
       </c>
       <c r="C24">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D24">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24">
         <v>21</v>
       </c>
       <c r="G24">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>39</v>
+        <v>0.75</v>
       </c>
       <c r="I24">
         <v>12</v>
       </c>
       <c r="J24">
+        <v>18</v>
+      </c>
+      <c r="K24" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>8</v>
+      </c>
+      <c r="N24">
+        <v>0.15</v>
+      </c>
+      <c r="O24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>70</v>
+      </c>
+      <c r="C25">
+        <v>30</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
+      </c>
+      <c r="E25">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>21</v>
+      </c>
+      <c r="G25">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25">
+        <v>12</v>
+      </c>
+      <c r="J25">
         <v>25</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
         <v>2</v>
       </c>
-      <c r="N24">
+      <c r="N25">
         <v>-0.2</v>
       </c>
-      <c r="O24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25">
-        <v>85</v>
-      </c>
-      <c r="C25">
-        <v>28</v>
-      </c>
-      <c r="D25">
-        <v>18</v>
-      </c>
-      <c r="E25">
-        <v>12</v>
-      </c>
-      <c r="F25">
-        <v>22</v>
-      </c>
-      <c r="I25">
-        <v>25</v>
-      </c>
-      <c r="J25">
-        <v>40</v>
-      </c>
-      <c r="L25">
-        <v>2</v>
-      </c>
-      <c r="M25">
-        <v>12</v>
-      </c>
       <c r="O25" t="s">
-        <v>105</v>
-      </c>
-      <c r="P25" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26">
-        <v>300</v>
+        <v>85</v>
       </c>
       <c r="C26">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D26">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E26">
-        <v>40</v>
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>22</v>
       </c>
       <c r="I26">
         <v>25</v>
@@ -1846,133 +1865,121 @@
         <v>40</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M26">
-        <v>14</v>
-      </c>
-      <c r="N26">
-        <v>0.2</v>
+        <v>12</v>
       </c>
       <c r="O26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>300</v>
+      </c>
+      <c r="C27">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+      <c r="E27">
+        <v>40</v>
+      </c>
+      <c r="I27">
+        <v>25</v>
+      </c>
+      <c r="J27">
+        <v>40</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>14</v>
+      </c>
+      <c r="N27">
+        <v>0.2</v>
+      </c>
+      <c r="O27" t="s">
+        <v>100</v>
+      </c>
+      <c r="P27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>15</v>
+      </c>
+      <c r="J28">
+        <v>25</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>5</v>
+      </c>
+      <c r="O28" t="s">
+        <v>89</v>
+      </c>
+      <c r="P28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
         <v>42</v>
       </c>
-      <c r="B27">
-        <v>30</v>
-      </c>
-      <c r="C27">
-        <v>16</v>
-      </c>
-      <c r="D27">
-        <v>15</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>15</v>
-      </c>
-      <c r="J27">
+      <c r="B29">
+        <v>80</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
         <v>25</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>5</v>
-      </c>
-      <c r="O27" t="s">
-        <v>93</v>
-      </c>
-      <c r="P27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28">
-        <v>80</v>
-      </c>
-      <c r="C28">
-        <v>40</v>
-      </c>
-      <c r="D28">
-        <v>25</v>
-      </c>
-      <c r="E28">
+      <c r="E29">
         <v>12</v>
-      </c>
-      <c r="F28">
-        <v>25</v>
-      </c>
-      <c r="G28">
-        <v>0.05</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I28">
-        <v>22</v>
-      </c>
-      <c r="J28">
-        <v>30</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>10</v>
-      </c>
-      <c r="O28" t="s">
-        <v>93</v>
-      </c>
-      <c r="P28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29">
-        <v>100</v>
-      </c>
-      <c r="C29">
-        <v>30</v>
-      </c>
-      <c r="D29">
-        <v>20</v>
-      </c>
-      <c r="E29">
-        <v>13</v>
       </c>
       <c r="F29">
         <v>25</v>
       </c>
       <c r="G29">
-        <v>0.5</v>
-      </c>
-      <c r="H29" t="s">
-        <v>46</v>
+        <v>0.05</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="I29">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J29">
-        <v>25</v>
-      </c>
-      <c r="K29" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -1980,124 +1987,133 @@
       <c r="M29">
         <v>10</v>
       </c>
-      <c r="N29">
-        <v>0.15</v>
-      </c>
       <c r="O29" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="P29" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C30">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D30">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E30">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F30">
         <v>25</v>
       </c>
       <c r="G30">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I30">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J30">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="K30" t="s">
+        <v>68</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="N30">
+        <v>0.15</v>
       </c>
       <c r="O30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="P30" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B31">
-        <v>300</v>
+        <v>95</v>
+      </c>
+      <c r="C31">
+        <v>36</v>
+      </c>
+      <c r="D31">
+        <v>24</v>
       </c>
       <c r="E31">
-        <v>50</v>
-      </c>
-      <c r="N31">
-        <v>0.25</v>
+        <v>14</v>
+      </c>
+      <c r="F31">
+        <v>25</v>
+      </c>
+      <c r="G31">
+        <v>0.2</v>
+      </c>
+      <c r="H31" t="s">
+        <v>47</v>
+      </c>
+      <c r="I31">
+        <v>26</v>
+      </c>
+      <c r="J31">
+        <v>36</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>16</v>
       </c>
       <c r="O31" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P31" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>300</v>
       </c>
-      <c r="C32">
-        <v>36</v>
-      </c>
-      <c r="D32">
-        <v>25</v>
-      </c>
       <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>20</v>
-      </c>
-      <c r="J32">
         <v>50</v>
       </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>15</v>
-      </c>
       <c r="N32">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="O32" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="P32" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B33">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C33">
         <v>36</v>
@@ -2109,13 +2125,10 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J33">
-        <v>30</v>
-      </c>
-      <c r="K33" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -2127,24 +2140,24 @@
         <v>0.2</v>
       </c>
       <c r="O33" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P33" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B34">
+        <v>200</v>
+      </c>
+      <c r="C34">
+        <v>36</v>
+      </c>
+      <c r="D34">
         <v>25</v>
-      </c>
-      <c r="C34">
-        <v>30</v>
-      </c>
-      <c r="D34">
-        <v>20</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -2155,17 +2168,58 @@
       <c r="J34">
         <v>30</v>
       </c>
+      <c r="K34" t="s">
+        <v>68</v>
+      </c>
       <c r="L34">
         <v>0</v>
       </c>
       <c r="M34">
+        <v>15</v>
+      </c>
+      <c r="N34">
+        <v>0.2</v>
+      </c>
+      <c r="O34" t="s">
+        <v>96</v>
+      </c>
+      <c r="P34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>20</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>22</v>
+      </c>
+      <c r="J35">
+        <v>30</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
         <v>8</v>
       </c>
-      <c r="O34" t="s">
-        <v>101</v>
-      </c>
-      <c r="P34" t="s">
-        <v>102</v>
+      <c r="O35" t="s">
+        <v>97</v>
+      </c>
+      <c r="P35" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.4.0 bug fix, new enemy ashes-skull, eyeball of the elder done.
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="117">
   <si>
     <t>NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -472,6 +472,21 @@
   <si>
     <t>POISON:0.2 ICE:-0.25</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AshesSkull</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIRE:0.3 SHADOW:0.2 HOLY:-0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNDEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NORMAL</t>
   </si>
 </sst>
 </file>
@@ -810,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1487,7 +1502,7 @@
         <v>6</v>
       </c>
       <c r="N17">
-        <v>-0.25</v>
+        <v>-0.2</v>
       </c>
       <c r="O17" t="s">
         <v>79</v>
@@ -1498,34 +1513,31 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>16</v>
+        <v>1000</v>
       </c>
       <c r="D18">
         <v>15</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18">
         <v>15</v>
       </c>
-      <c r="G18">
-        <v>0.15</v>
-      </c>
-      <c r="H18" t="s">
-        <v>27</v>
-      </c>
       <c r="I18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J18">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="K18" t="s">
+        <v>116</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1533,116 +1545,125 @@
       <c r="M18">
         <v>5</v>
       </c>
+      <c r="N18">
+        <v>0.3</v>
+      </c>
       <c r="O18" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="P18" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="B19">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C19">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>15</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19">
         <v>15</v>
       </c>
       <c r="G19">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="H19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J19">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>20</v>
       </c>
       <c r="D20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>0.125</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>32</v>
+        <v>0.2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>29</v>
       </c>
       <c r="I20">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J20">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B21">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D21">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E21">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
       </c>
       <c r="G21">
-        <v>0.33329999999999999</v>
+        <v>0.125</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J21">
         <v>25</v>
@@ -1651,247 +1672,250 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>10</v>
-      </c>
-      <c r="N21">
-        <v>0.25</v>
+        <v>6</v>
       </c>
       <c r="O21" t="s">
-        <v>82</v>
-      </c>
-      <c r="P21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>200</v>
+      </c>
+      <c r="C22">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22">
+        <v>20</v>
+      </c>
+      <c r="J22">
+        <v>25</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>10</v>
+      </c>
+      <c r="N22">
+        <v>0.25</v>
+      </c>
+      <c r="O22" t="s">
+        <v>82</v>
+      </c>
+      <c r="P22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>35</v>
-      </c>
-      <c r="B22">
-        <v>65</v>
-      </c>
-      <c r="C22">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>20</v>
-      </c>
-      <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="F22">
-        <v>20</v>
-      </c>
-      <c r="G22">
-        <v>0.1</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22">
-        <v>16</v>
-      </c>
-      <c r="J22">
-        <v>26</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>5</v>
-      </c>
-      <c r="N22">
-        <v>0.2</v>
-      </c>
-      <c r="O22" t="s">
-        <v>84</v>
-      </c>
-      <c r="P22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>13</v>
       </c>
       <c r="B23">
         <v>65</v>
       </c>
       <c r="C23">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D23">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E23">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G23">
-        <v>0.3</v>
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="I23">
         <v>16</v>
       </c>
       <c r="J23">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="N23">
+        <v>0.2</v>
       </c>
       <c r="O23" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="P23" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B24">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C24">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D24">
         <v>18</v>
       </c>
       <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24">
+        <v>0.3</v>
+      </c>
+      <c r="I24">
+        <v>16</v>
+      </c>
+      <c r="J24">
+        <v>30</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
         <v>10</v>
       </c>
-      <c r="F24">
-        <v>21</v>
-      </c>
-      <c r="G24">
-        <v>0.75</v>
-      </c>
-      <c r="I24">
-        <v>12</v>
-      </c>
-      <c r="J24">
-        <v>18</v>
-      </c>
-      <c r="K24" t="s">
-        <v>68</v>
-      </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="M24">
-        <v>8</v>
-      </c>
-      <c r="N24">
-        <v>0.15</v>
-      </c>
       <c r="O24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+        <v>102</v>
+      </c>
+      <c r="P24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B25">
         <v>70</v>
       </c>
       <c r="C25">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D25">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25">
         <v>21</v>
       </c>
       <c r="G25">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>38</v>
+        <v>0.75</v>
       </c>
       <c r="I25">
         <v>12</v>
       </c>
       <c r="J25">
+        <v>18</v>
+      </c>
+      <c r="K25" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>8</v>
+      </c>
+      <c r="N25">
+        <v>0.15</v>
+      </c>
+      <c r="O25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>70</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+      <c r="F26">
+        <v>21</v>
+      </c>
+      <c r="G26">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26">
+        <v>12</v>
+      </c>
+      <c r="J26">
         <v>25</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
         <v>2</v>
       </c>
-      <c r="N25">
+      <c r="N26">
         <v>-0.2</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O26" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26">
-        <v>85</v>
-      </c>
-      <c r="C26">
-        <v>28</v>
-      </c>
-      <c r="D26">
-        <v>18</v>
-      </c>
-      <c r="E26">
-        <v>12</v>
-      </c>
-      <c r="F26">
-        <v>22</v>
-      </c>
-      <c r="I26">
-        <v>25</v>
-      </c>
-      <c r="J26">
-        <v>40</v>
-      </c>
-      <c r="L26">
-        <v>2</v>
-      </c>
-      <c r="M26">
-        <v>12</v>
-      </c>
-      <c r="O26" t="s">
-        <v>101</v>
-      </c>
-      <c r="P26" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
-        <v>300</v>
+        <v>85</v>
       </c>
       <c r="C27">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D27">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E27">
-        <v>40</v>
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>22</v>
       </c>
       <c r="I27">
         <v>25</v>
@@ -1900,133 +1924,121 @@
         <v>40</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M27">
-        <v>14</v>
-      </c>
-      <c r="N27">
-        <v>0.2</v>
+        <v>12</v>
       </c>
       <c r="O27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>300</v>
+      </c>
+      <c r="C28">
+        <v>32</v>
+      </c>
+      <c r="D28">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>40</v>
+      </c>
+      <c r="I28">
+        <v>25</v>
+      </c>
+      <c r="J28">
+        <v>40</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>14</v>
+      </c>
+      <c r="N28">
+        <v>0.2</v>
+      </c>
+      <c r="O28" t="s">
+        <v>100</v>
+      </c>
+      <c r="P28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>30</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>16</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>15</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="I28">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>15</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <v>25</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
         <v>5</v>
-      </c>
-      <c r="O28" t="s">
-        <v>89</v>
-      </c>
-      <c r="P28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29">
-        <v>80</v>
-      </c>
-      <c r="C29">
-        <v>40</v>
-      </c>
-      <c r="D29">
-        <v>25</v>
-      </c>
-      <c r="E29">
-        <v>12</v>
-      </c>
-      <c r="F29">
-        <v>25</v>
-      </c>
-      <c r="G29">
-        <v>0.05</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I29">
-        <v>22</v>
-      </c>
-      <c r="J29">
-        <v>30</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>10</v>
       </c>
       <c r="O29" t="s">
         <v>89</v>
       </c>
       <c r="P29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C30">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D30">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E30">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F30">
         <v>25</v>
       </c>
       <c r="G30">
-        <v>0.5</v>
-      </c>
-      <c r="H30" t="s">
-        <v>45</v>
+        <v>0.05</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="I30">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J30">
-        <v>25</v>
-      </c>
-      <c r="K30" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -2034,124 +2046,133 @@
       <c r="M30">
         <v>10</v>
       </c>
-      <c r="N30">
-        <v>0.15</v>
-      </c>
       <c r="O30" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="P30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B31">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C31">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D31">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E31">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F31">
         <v>25</v>
       </c>
       <c r="G31">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I31">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J31">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="K31" t="s">
+        <v>68</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="N31">
+        <v>0.15</v>
       </c>
       <c r="O31" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="P31" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32">
-        <v>300</v>
+        <v>95</v>
+      </c>
+      <c r="C32">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>24</v>
       </c>
       <c r="E32">
-        <v>50</v>
-      </c>
-      <c r="N32">
-        <v>0.25</v>
+        <v>14</v>
+      </c>
+      <c r="F32">
+        <v>25</v>
+      </c>
+      <c r="G32">
+        <v>0.2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32">
+        <v>26</v>
+      </c>
+      <c r="J32">
+        <v>36</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>16</v>
       </c>
       <c r="O32" t="s">
         <v>92</v>
       </c>
       <c r="P32" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33">
         <v>300</v>
       </c>
-      <c r="C33">
-        <v>36</v>
-      </c>
-      <c r="D33">
-        <v>25</v>
-      </c>
       <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>20</v>
-      </c>
-      <c r="J33">
         <v>50</v>
       </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>15</v>
-      </c>
       <c r="N33">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="O33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C34">
         <v>36</v>
@@ -2163,13 +2184,10 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J34">
-        <v>30</v>
-      </c>
-      <c r="K34" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -2181,7 +2199,7 @@
         <v>0.2</v>
       </c>
       <c r="O34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P34" t="s">
         <v>94</v>
@@ -2189,16 +2207,16 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35">
+        <v>200</v>
+      </c>
+      <c r="C35">
+        <v>36</v>
+      </c>
+      <c r="D35">
         <v>25</v>
-      </c>
-      <c r="C35">
-        <v>30</v>
-      </c>
-      <c r="D35">
-        <v>20</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2209,16 +2227,57 @@
       <c r="J35">
         <v>30</v>
       </c>
+      <c r="K35" t="s">
+        <v>68</v>
+      </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
+        <v>15</v>
+      </c>
+      <c r="N35">
+        <v>0.2</v>
+      </c>
+      <c r="O35" t="s">
+        <v>96</v>
+      </c>
+      <c r="P35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>25</v>
+      </c>
+      <c r="C36">
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <v>20</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>22</v>
+      </c>
+      <c r="J36">
+        <v>30</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
         <v>8</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O36" t="s">
         <v>97</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P36" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.4.0 finally convert Level to kotlin, manifest commit.
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
   <si>
     <t>NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -342,10 +342,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SHADOW:0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>POISON:0.25</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -410,83 +406,91 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>DEMONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIGHT:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIGHT:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GreatCrab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MINIBOSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIRE:-0.25 POISON:0.2 HOLY:-0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NewbornElemental</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEMONIC MINIBOSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIGHT:0.25 POISON:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW:0.2 HOLY:-0.25 POISON:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW:0.2 FIRE:-0.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON:0.2 ICE:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AshesSkull</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIRE:0.3 SHADOW:0.2 HOLY:-0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNDEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>SHADOW:0.2 POISON:-0.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICE:-0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW:0.2 POISON:0.15 FIRE:0.15 HOLY:-0.2 ICE:-0.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>POISON:0.2 HOLY:-0.25</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMONIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2 POISON:0.15 FIRE:0.15 HOLY:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIGHT:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIGHT:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GreatCrab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MINIBOSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIRE:-0.25 POISON:0.2 HOLY:-0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NewbornElemental</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMONIC MINIBOSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIGHT:0.25 POISON:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2 HOLY:-0.25 POISON:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2 FIRE:-0.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 ICE:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AshesSkull</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIRE:0.3 SHADOW:0.2 HOLY:-0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UNDEAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NORMAL</t>
   </si>
 </sst>
 </file>
@@ -828,7 +832,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1082,13 +1086,16 @@
       <c r="M6">
         <v>2</v>
       </c>
+      <c r="O6" t="s">
+        <v>115</v>
+      </c>
       <c r="P6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B7">
         <v>25</v>
@@ -1124,7 +1131,7 @@
         <v>69</v>
       </c>
       <c r="P7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
@@ -1156,7 +1163,7 @@
         <v>0.25</v>
       </c>
       <c r="O8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="P8" t="s">
         <v>72</v>
@@ -1266,6 +1273,9 @@
       <c r="M11">
         <v>3</v>
       </c>
+      <c r="N11">
+        <v>0.15</v>
+      </c>
       <c r="O11" t="s">
         <v>71</v>
       </c>
@@ -1314,7 +1324,7 @@
         <v>0.15</v>
       </c>
       <c r="O12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.15">
@@ -1351,6 +1361,9 @@
       <c r="M13">
         <v>6</v>
       </c>
+      <c r="N13">
+        <v>-0.2</v>
+      </c>
       <c r="O13" t="s">
         <v>76</v>
       </c>
@@ -1377,6 +1390,9 @@
       <c r="M14">
         <v>5</v>
       </c>
+      <c r="N14">
+        <v>0.5</v>
+      </c>
       <c r="O14" t="s">
         <v>62</v>
       </c>
@@ -1386,7 +1402,7 @@
     </row>
     <row r="15" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B15">
         <v>65</v>
@@ -1420,10 +1436,10 @@
         <v>0.2</v>
       </c>
       <c r="O15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">
@@ -1446,7 +1462,7 @@
         <v>6</v>
       </c>
       <c r="J16">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1458,7 +1474,7 @@
         <v>0.25</v>
       </c>
       <c r="O16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P16" t="s">
         <v>77</v>
@@ -1513,7 +1529,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B18">
         <v>20</v>
@@ -1537,7 +1553,7 @@
         <v>12</v>
       </c>
       <c r="K18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1549,15 +1565,15 @@
         <v>0.3</v>
       </c>
       <c r="O18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="P18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B19">
         <v>30</v>
@@ -1593,7 +1609,7 @@
         <v>5</v>
       </c>
       <c r="O19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
@@ -1634,7 +1650,7 @@
         <v>8</v>
       </c>
       <c r="O20" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
@@ -1675,7 +1691,7 @@
         <v>6</v>
       </c>
       <c r="O21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
@@ -1716,10 +1732,10 @@
         <v>0.25</v>
       </c>
       <c r="O22" t="s">
+        <v>81</v>
+      </c>
+      <c r="P22" t="s">
         <v>82</v>
-      </c>
-      <c r="P22" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
@@ -1763,7 +1779,7 @@
         <v>0.2</v>
       </c>
       <c r="O23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P23" t="s">
         <v>75</v>
@@ -1804,10 +1820,10 @@
         <v>10</v>
       </c>
       <c r="O24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
@@ -1851,7 +1867,7 @@
         <v>0.15</v>
       </c>
       <c r="O25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
@@ -1930,10 +1946,10 @@
         <v>12</v>
       </c>
       <c r="O27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="P27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
@@ -1968,10 +1984,10 @@
         <v>0.2</v>
       </c>
       <c r="O28" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="P28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
@@ -2003,10 +2019,10 @@
         <v>5</v>
       </c>
       <c r="O29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
@@ -2047,10 +2063,10 @@
         <v>10</v>
       </c>
       <c r="O30" t="s">
+        <v>88</v>
+      </c>
+      <c r="P30" t="s">
         <v>89</v>
-      </c>
-      <c r="P30" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
@@ -2097,10 +2113,10 @@
         <v>0.15</v>
       </c>
       <c r="O31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="P31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
@@ -2140,8 +2156,11 @@
       <c r="M32">
         <v>16</v>
       </c>
+      <c r="N32">
+        <v>-0.25</v>
+      </c>
       <c r="O32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P32" t="s">
         <v>56</v>
@@ -2161,10 +2180,10 @@
         <v>0.25</v>
       </c>
       <c r="O33" t="s">
+        <v>91</v>
+      </c>
+      <c r="P33" t="s">
         <v>92</v>
-      </c>
-      <c r="P33" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.15">
@@ -2199,10 +2218,10 @@
         <v>0.2</v>
       </c>
       <c r="O34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.15">
@@ -2240,10 +2259,10 @@
         <v>0.2</v>
       </c>
       <c r="O35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.15">
@@ -2274,11 +2293,14 @@
       <c r="M36">
         <v>8</v>
       </c>
+      <c r="N36">
+        <v>-0.15</v>
+      </c>
       <c r="O36" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="P36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.4.1 serveral perks, damage wand changing.
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -832,7 +832,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1802,7 +1802,7 @@
         <v>12</v>
       </c>
       <c r="F24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24">
         <v>0.3</v>
@@ -2086,7 +2086,7 @@
         <v>13</v>
       </c>
       <c r="F31">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G31">
         <v>0.5</v>
@@ -2136,7 +2136,7 @@
         <v>14</v>
       </c>
       <c r="F32">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G32">
         <v>0.2</v>

</xml_diff>

<commit_message>
0.4.1 add prize trap, now ready for prerelease.
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -832,7 +832,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -999,7 +999,7 @@
         <v>15</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4">
         <v>8</v>
@@ -1538,7 +1538,7 @@
         <v>1000</v>
       </c>
       <c r="D18">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>6</v>
@@ -1559,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N18">
         <v>0.3</v>

</xml_diff>

<commit_message>
0.4.2 rare enemy quick-firing gun.
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gamemaker\projects\pixel-dungeon\dpd\darkest-pixel-dungeon\dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\the_gamemaker\Projects\PixelDungeon\dpd\darkest-pixel-dungeon\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
   <si>
     <t>NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -490,6 +490,10 @@
   </si>
   <si>
     <t>POISON:0.2 HOLY:-0.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuickFiringGun</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -829,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1828,145 +1832,151 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B25">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D25">
         <v>18</v>
       </c>
       <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>22</v>
+      </c>
+      <c r="G25">
+        <v>0.3</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>12</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
         <v>10</v>
       </c>
-      <c r="F25">
-        <v>21</v>
-      </c>
-      <c r="G25">
-        <v>0.75</v>
-      </c>
-      <c r="I25">
-        <v>12</v>
-      </c>
-      <c r="J25">
-        <v>18</v>
-      </c>
-      <c r="K25" t="s">
-        <v>68</v>
-      </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-      <c r="M25">
-        <v>8</v>
-      </c>
-      <c r="N25">
-        <v>0.15</v>
-      </c>
       <c r="O25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+        <v>98</v>
+      </c>
+      <c r="P25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B26">
         <v>70</v>
       </c>
       <c r="C26">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D26">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E26">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26">
         <v>21</v>
       </c>
       <c r="G26">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>38</v>
+        <v>0.75</v>
       </c>
       <c r="I26">
         <v>12</v>
       </c>
       <c r="J26">
+        <v>18</v>
+      </c>
+      <c r="K26" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>8</v>
+      </c>
+      <c r="N26">
+        <v>0.15</v>
+      </c>
+      <c r="O26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27">
+        <v>70</v>
+      </c>
+      <c r="C27">
+        <v>30</v>
+      </c>
+      <c r="D27">
+        <v>30</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+      <c r="F27">
+        <v>21</v>
+      </c>
+      <c r="G27">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27">
+        <v>12</v>
+      </c>
+      <c r="J27">
         <v>25</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
         <v>2</v>
       </c>
-      <c r="N26">
+      <c r="N27">
         <v>-0.2</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O27" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27">
-        <v>85</v>
-      </c>
-      <c r="C27">
-        <v>28</v>
-      </c>
-      <c r="D27">
-        <v>18</v>
-      </c>
-      <c r="E27">
-        <v>12</v>
-      </c>
-      <c r="F27">
-        <v>22</v>
-      </c>
-      <c r="I27">
-        <v>25</v>
-      </c>
-      <c r="J27">
-        <v>40</v>
-      </c>
-      <c r="L27">
-        <v>2</v>
-      </c>
-      <c r="M27">
-        <v>12</v>
-      </c>
-      <c r="O27" t="s">
-        <v>98</v>
-      </c>
-      <c r="P27" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28">
-        <v>300</v>
+        <v>85</v>
       </c>
       <c r="C28">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D28">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E28">
-        <v>40</v>
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>22</v>
       </c>
       <c r="I28">
         <v>25</v>
@@ -1975,133 +1985,121 @@
         <v>40</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M28">
-        <v>14</v>
-      </c>
-      <c r="N28">
-        <v>0.2</v>
+        <v>12</v>
       </c>
       <c r="O28" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="P28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>300</v>
+      </c>
+      <c r="C29">
+        <v>32</v>
+      </c>
+      <c r="D29">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>40</v>
+      </c>
+      <c r="I29">
+        <v>25</v>
+      </c>
+      <c r="J29">
+        <v>40</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>14</v>
+      </c>
+      <c r="N29">
+        <v>0.2</v>
+      </c>
+      <c r="O29" t="s">
+        <v>116</v>
+      </c>
+      <c r="P29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
         <v>41</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>30</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>16</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>15</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="I29">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="I30">
         <v>15</v>
       </c>
-      <c r="J29">
+      <c r="J30">
         <v>25</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
         <v>5</v>
-      </c>
-      <c r="O29" t="s">
-        <v>88</v>
-      </c>
-      <c r="P29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30">
-        <v>80</v>
-      </c>
-      <c r="C30">
-        <v>40</v>
-      </c>
-      <c r="D30">
-        <v>25</v>
-      </c>
-      <c r="E30">
-        <v>12</v>
-      </c>
-      <c r="F30">
-        <v>25</v>
-      </c>
-      <c r="G30">
-        <v>0.05</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I30">
-        <v>22</v>
-      </c>
-      <c r="J30">
-        <v>30</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>10</v>
       </c>
       <c r="O30" t="s">
         <v>88</v>
       </c>
       <c r="P30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B31">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C31">
+        <v>40</v>
+      </c>
+      <c r="D31">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>12</v>
+      </c>
+      <c r="F31">
+        <v>25</v>
+      </c>
+      <c r="G31">
+        <v>0.05</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31">
+        <v>22</v>
+      </c>
+      <c r="J31">
         <v>30</v>
-      </c>
-      <c r="D31">
-        <v>20</v>
-      </c>
-      <c r="E31">
-        <v>13</v>
-      </c>
-      <c r="F31">
-        <v>26</v>
-      </c>
-      <c r="G31">
-        <v>0.5</v>
-      </c>
-      <c r="H31" t="s">
-        <v>45</v>
-      </c>
-      <c r="I31">
-        <v>15</v>
-      </c>
-      <c r="J31">
-        <v>25</v>
-      </c>
-      <c r="K31" t="s">
-        <v>68</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -2109,127 +2107,136 @@
       <c r="M31">
         <v>10</v>
       </c>
-      <c r="N31">
-        <v>0.15</v>
-      </c>
       <c r="O31" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="P31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C32">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D32">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E32">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32">
         <v>26</v>
       </c>
       <c r="G32">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I32">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J32">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="K32" t="s">
+        <v>68</v>
       </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="N32">
-        <v>-0.25</v>
+        <v>0.15</v>
       </c>
       <c r="O32" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="P32" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33">
-        <v>300</v>
+        <v>95</v>
+      </c>
+      <c r="C33">
+        <v>36</v>
+      </c>
+      <c r="D33">
+        <v>24</v>
       </c>
       <c r="E33">
-        <v>50</v>
+        <v>14</v>
+      </c>
+      <c r="F33">
+        <v>26</v>
+      </c>
+      <c r="G33">
+        <v>0.2</v>
+      </c>
+      <c r="H33" t="s">
+        <v>47</v>
+      </c>
+      <c r="I33">
+        <v>26</v>
+      </c>
+      <c r="J33">
+        <v>36</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>16</v>
       </c>
       <c r="N33">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="O33" t="s">
         <v>91</v>
       </c>
       <c r="P33" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>300</v>
       </c>
-      <c r="C34">
-        <v>36</v>
-      </c>
-      <c r="D34">
-        <v>25</v>
-      </c>
       <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>20</v>
-      </c>
-      <c r="J34">
         <v>50</v>
       </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <v>15</v>
-      </c>
       <c r="N34">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="O34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="P34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C35">
         <v>36</v>
@@ -2241,13 +2248,10 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J35">
-        <v>30</v>
-      </c>
-      <c r="K35" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -2259,7 +2263,7 @@
         <v>0.2</v>
       </c>
       <c r="O35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P35" t="s">
         <v>93</v>
@@ -2267,16 +2271,16 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36">
+        <v>200</v>
+      </c>
+      <c r="C36">
+        <v>36</v>
+      </c>
+      <c r="D36">
         <v>25</v>
-      </c>
-      <c r="C36">
-        <v>30</v>
-      </c>
-      <c r="D36">
-        <v>20</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -2287,19 +2291,60 @@
       <c r="J36">
         <v>30</v>
       </c>
+      <c r="K36" t="s">
+        <v>68</v>
+      </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
+        <v>15</v>
+      </c>
+      <c r="N36">
+        <v>0.2</v>
+      </c>
+      <c r="O36" t="s">
+        <v>95</v>
+      </c>
+      <c r="P36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>22</v>
+      </c>
+      <c r="J37">
+        <v>30</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
         <v>8</v>
       </c>
-      <c r="N36">
+      <c r="N37">
         <v>-0.15</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O37" t="s">
         <v>117</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P37" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.4.2 working on rings, ring of evasion changed.
</commit_message>
<xml_diff>
--- a/dev/mobs.xlsx
+++ b/dev/mobs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
   <si>
     <t>NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -232,10 +232,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>elementalResistance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Thief</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -271,10 +267,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>POISON:0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IMMOVABLE MINIBOSS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -283,10 +275,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SHADOW:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>atkSkill</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -298,26 +286,10 @@
     <t>MAGICAL</t>
   </si>
   <si>
-    <t>LIGHT:-0.2 ICE:0.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 HOLY:-0.25 SHADOW:0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BOSS DEMONIC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FIRE:-0.3 HOLY:-0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>UNDEAD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -326,10 +298,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BOSS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -338,26 +306,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FIRE:-0.25 SHADOW:0.25 HOLY:-0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICE:-0.15 POISON:0.3 LIGHT:-0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BOSS MACHINE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FIRE:0.5 HOLY:-0.2 ICE:-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MACHINE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -374,10 +326,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SHADOW:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DEMONIC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -386,10 +334,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>POISON:0.2 SHADOW:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BOSS DEMONIC IMMOVABLE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -398,30 +342,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>POISON:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 SHADOW:0.2 HOLY:-0.25 ICE:-0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DEMONIC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIGHT:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIGHT:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GreatCrab</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -430,10 +354,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FIRE:-0.25 POISON:0.2 HOLY:-0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NewbornElemental</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -442,34 +362,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LIGHT:0.25 POISON:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2 HOLY:-0.25 POISON:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Bat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SHADOW:0.2 FIRE:-0.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 ICE:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AshesSkull</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FIRE:0.3 SHADOW:0.2 HOLY:-0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>UNDEAD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -477,23 +377,31 @@
     <t>NORMAL</t>
   </si>
   <si>
-    <t>SHADOW:0.2 POISON:-0.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICE:-0.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHADOW:0.2 POISON:0.15 FIRE:0.15 HOLY:-0.2 ICE:-0.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POISON:0.2 HOLY:-0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>QuickFiringGun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIRE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POISON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIGHT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHADOW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOLY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -833,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -845,19 +753,23 @@
     <col min="3" max="3" width="12.125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="7" max="7" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="19.375" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="11.625" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
     <col min="11" max="11" width="12.625" customWidth="1"/>
     <col min="12" max="12" width="10.875" customWidth="1"/>
     <col min="13" max="13" width="10.75" customWidth="1"/>
-    <col min="14" max="14" width="18.125" customWidth="1"/>
-    <col min="15" max="15" width="26.375" customWidth="1"/>
-    <col min="16" max="16" width="24.75" customWidth="1"/>
-    <col min="17" max="17" width="16.125" customWidth="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1"/>
+    <col min="15" max="15" width="9.25" customWidth="1"/>
+    <col min="16" max="16" width="9.625" customWidth="1"/>
+    <col min="17" max="17" width="9.5" customWidth="1"/>
+    <col min="18" max="18" width="10.125" customWidth="1"/>
+    <col min="20" max="20" width="8.875" customWidth="1"/>
+    <col min="21" max="21" width="24.75" customWidth="1"/>
+    <col min="22" max="22" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -865,10 +777,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -901,13 +813,28 @@
         <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="P1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+        <v>91</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -938,8 +865,14 @@
       <c r="M2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O2">
+        <v>-0.3</v>
+      </c>
+      <c r="P2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -977,12 +910,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -1014,13 +947,19 @@
       <c r="M4">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="N4">
+        <v>-0.2</v>
+      </c>
+      <c r="Q4">
+        <v>0.1</v>
+      </c>
+      <c r="R4">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -1049,16 +988,22 @@
       <c r="M5">
         <v>2</v>
       </c>
-      <c r="O5" t="s">
-        <v>70</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="P5">
+        <v>0.2</v>
+      </c>
+      <c r="S5">
+        <v>0.2</v>
+      </c>
+      <c r="T5">
+        <v>-0.25</v>
+      </c>
+      <c r="U5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>59</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -1090,16 +1035,16 @@
       <c r="M6">
         <v>2</v>
       </c>
-      <c r="O6" t="s">
-        <v>115</v>
-      </c>
-      <c r="P6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q6">
+        <v>-0.2</v>
+      </c>
+      <c r="U6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="B7">
         <v>25</v>
@@ -1131,14 +1076,17 @@
       <c r="M7">
         <v>4</v>
       </c>
-      <c r="O7" t="s">
-        <v>69</v>
-      </c>
-      <c r="P7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q7">
+        <v>0.1</v>
+      </c>
+      <c r="R7">
+        <v>-0.2</v>
+      </c>
+      <c r="U7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1166,14 +1114,20 @@
       <c r="N8">
         <v>0.25</v>
       </c>
-      <c r="O8" t="s">
-        <v>102</v>
-      </c>
-      <c r="P8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O8">
+        <v>-0.25</v>
+      </c>
+      <c r="P8">
+        <v>0.2</v>
+      </c>
+      <c r="T8">
+        <v>-0.3</v>
+      </c>
+      <c r="U8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1199,7 +1153,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1233,16 +1187,19 @@
       <c r="M10">
         <v>2</v>
       </c>
-      <c r="O10" t="s">
-        <v>73</v>
-      </c>
-      <c r="P10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="O10">
+        <v>-0.3</v>
+      </c>
+      <c r="T10">
+        <v>-0.3</v>
+      </c>
+      <c r="U10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -1263,7 +1220,7 @@
         <v>0.01</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1280,14 +1237,20 @@
       <c r="N11">
         <v>0.15</v>
       </c>
-      <c r="O11" t="s">
-        <v>71</v>
-      </c>
-      <c r="P11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P11">
+        <v>0.2</v>
+      </c>
+      <c r="Q11">
+        <v>-0.15</v>
+      </c>
+      <c r="T11">
+        <v>-0.2</v>
+      </c>
+      <c r="U11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1316,7 +1279,7 @@
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1327,11 +1290,20 @@
       <c r="N12">
         <v>0.15</v>
       </c>
-      <c r="O12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O12">
+        <v>0.1</v>
+      </c>
+      <c r="P12">
+        <v>-0.2</v>
+      </c>
+      <c r="Q12">
+        <v>0.2</v>
+      </c>
+      <c r="R12">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1368,16 +1340,13 @@
       <c r="N13">
         <v>-0.2</v>
       </c>
-      <c r="O13" t="s">
-        <v>76</v>
-      </c>
-      <c r="P13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="U13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14">
         <v>80</v>
@@ -1397,16 +1366,16 @@
       <c r="N14">
         <v>0.5</v>
       </c>
-      <c r="O14" t="s">
-        <v>62</v>
-      </c>
-      <c r="P14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="P14">
+        <v>0.5</v>
+      </c>
+      <c r="U14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>65</v>
@@ -1439,14 +1408,20 @@
       <c r="N15">
         <v>0.2</v>
       </c>
-      <c r="O15" t="s">
-        <v>83</v>
-      </c>
-      <c r="P15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O15">
+        <v>0.5</v>
+      </c>
+      <c r="Q15">
+        <v>-1</v>
+      </c>
+      <c r="T15">
+        <v>-0.25</v>
+      </c>
+      <c r="U15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1477,14 +1452,17 @@
       <c r="N16">
         <v>0.25</v>
       </c>
-      <c r="O16" t="s">
-        <v>109</v>
-      </c>
-      <c r="P16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P16">
+        <v>0.2</v>
+      </c>
+      <c r="Q16">
+        <v>-0.25</v>
+      </c>
+      <c r="U16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1524,16 +1502,22 @@
       <c r="N17">
         <v>-0.2</v>
       </c>
-      <c r="O17" t="s">
-        <v>79</v>
-      </c>
-      <c r="P17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O17">
+        <v>-0.25</v>
+      </c>
+      <c r="S17">
+        <v>0.25</v>
+      </c>
+      <c r="T17">
+        <v>-0.3</v>
+      </c>
+      <c r="U17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="B18">
         <v>20</v>
@@ -1557,7 +1541,7 @@
         <v>12</v>
       </c>
       <c r="K18" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1568,16 +1552,25 @@
       <c r="N18">
         <v>0.3</v>
       </c>
-      <c r="O18" t="s">
-        <v>111</v>
-      </c>
-      <c r="P18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O18">
+        <v>0.3</v>
+      </c>
+      <c r="Q18">
+        <v>-0.2</v>
+      </c>
+      <c r="S18">
+        <v>0.2</v>
+      </c>
+      <c r="T18">
+        <v>-0.3</v>
+      </c>
+      <c r="U18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B19">
         <v>30</v>
@@ -1612,11 +1605,20 @@
       <c r="M19">
         <v>5</v>
       </c>
-      <c r="O19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O19">
+        <v>-0.15</v>
+      </c>
+      <c r="Q19">
+        <v>0.3</v>
+      </c>
+      <c r="S19">
+        <v>0.2</v>
+      </c>
+      <c r="T19">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1653,11 +1655,14 @@
       <c r="M20">
         <v>8</v>
       </c>
-      <c r="O20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="P20">
+        <v>-0.15</v>
+      </c>
+      <c r="S20">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1694,11 +1699,14 @@
       <c r="M21">
         <v>6</v>
       </c>
-      <c r="O21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="O21">
+        <v>-0.2</v>
+      </c>
+      <c r="P21">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1735,14 +1743,20 @@
       <c r="N22">
         <v>0.25</v>
       </c>
-      <c r="O22" t="s">
-        <v>81</v>
-      </c>
-      <c r="P22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="P22">
+        <v>0.3</v>
+      </c>
+      <c r="Q22">
+        <v>0.1</v>
+      </c>
+      <c r="R22">
+        <v>-0.25</v>
+      </c>
+      <c r="U22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1782,14 +1796,20 @@
       <c r="N23">
         <v>0.2</v>
       </c>
-      <c r="O23" t="s">
-        <v>83</v>
-      </c>
-      <c r="P23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O23">
+        <v>0.5</v>
+      </c>
+      <c r="Q23">
+        <v>-1</v>
+      </c>
+      <c r="T23">
+        <v>-0.2</v>
+      </c>
+      <c r="U23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1823,16 +1843,19 @@
       <c r="M24">
         <v>10</v>
       </c>
-      <c r="O24" t="s">
-        <v>99</v>
-      </c>
-      <c r="P24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q24">
+        <v>0.1</v>
+      </c>
+      <c r="R24">
+        <v>-0.2</v>
+      </c>
+      <c r="U24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B25">
         <v>65</v>
@@ -1864,16 +1887,19 @@
       <c r="M25">
         <v>10</v>
       </c>
-      <c r="O25" t="s">
-        <v>98</v>
-      </c>
-      <c r="P25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q25">
+        <v>0.1</v>
+      </c>
+      <c r="R25">
+        <v>-0.2</v>
+      </c>
+      <c r="U25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26">
         <v>70</v>
@@ -1900,7 +1926,7 @@
         <v>18</v>
       </c>
       <c r="K26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -1911,11 +1937,17 @@
       <c r="N26">
         <v>0.15</v>
       </c>
-      <c r="O26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="P26">
+        <v>-0.2</v>
+      </c>
+      <c r="S26">
+        <v>0.2</v>
+      </c>
+      <c r="T26">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1955,11 +1987,17 @@
       <c r="N27">
         <v>-0.2</v>
       </c>
-      <c r="O27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q27">
+        <v>-0.15</v>
+      </c>
+      <c r="S27">
+        <v>0.2</v>
+      </c>
+      <c r="T27">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1990,19 +2028,22 @@
       <c r="M28">
         <v>12</v>
       </c>
-      <c r="O28" t="s">
-        <v>98</v>
-      </c>
-      <c r="P28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q28">
+        <v>0.2</v>
+      </c>
+      <c r="R28">
+        <v>-0.2</v>
+      </c>
+      <c r="U28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>40</v>
       </c>
       <c r="B29">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C29">
         <v>32</v>
@@ -2028,14 +2069,26 @@
       <c r="N29">
         <v>0.2</v>
       </c>
-      <c r="O29" t="s">
-        <v>116</v>
-      </c>
-      <c r="P29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O29">
+        <v>0.15</v>
+      </c>
+      <c r="P29">
+        <v>0.15</v>
+      </c>
+      <c r="Q29">
+        <v>-0.15</v>
+      </c>
+      <c r="S29">
+        <v>0.2</v>
+      </c>
+      <c r="T29">
+        <v>-0.2</v>
+      </c>
+      <c r="U29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2066,14 +2119,23 @@
       <c r="N30">
         <v>-0.15</v>
       </c>
-      <c r="O30" t="s">
-        <v>88</v>
-      </c>
-      <c r="P30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="O30">
+        <v>-0.3</v>
+      </c>
+      <c r="R30">
+        <v>0.15</v>
+      </c>
+      <c r="S30">
+        <v>0.2</v>
+      </c>
+      <c r="T30">
+        <v>-0.4</v>
+      </c>
+      <c r="U30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2110,14 +2172,23 @@
       <c r="M31">
         <v>10</v>
       </c>
-      <c r="O31" t="s">
-        <v>88</v>
-      </c>
-      <c r="P31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q31">
+        <v>-0.2</v>
+      </c>
+      <c r="R31">
+        <v>-0.2</v>
+      </c>
+      <c r="S31">
+        <v>0.2</v>
+      </c>
+      <c r="T31">
+        <v>-0.25</v>
+      </c>
+      <c r="U31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2149,7 +2220,7 @@
         <v>25</v>
       </c>
       <c r="K32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -2160,14 +2231,14 @@
       <c r="N32">
         <v>0.15</v>
       </c>
-      <c r="O32" t="s">
-        <v>97</v>
-      </c>
-      <c r="P32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="T32">
+        <v>-0.25</v>
+      </c>
+      <c r="U32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -2207,14 +2278,23 @@
       <c r="N33">
         <v>-0.25</v>
       </c>
-      <c r="O33" t="s">
-        <v>91</v>
-      </c>
-      <c r="P33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P33">
+        <v>0.2</v>
+      </c>
+      <c r="Q33">
+        <v>-0.25</v>
+      </c>
+      <c r="S33">
+        <v>0.2</v>
+      </c>
+      <c r="T33">
+        <v>-0.2</v>
+      </c>
+      <c r="U33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2227,14 +2307,20 @@
       <c r="N34">
         <v>0.25</v>
       </c>
-      <c r="O34" t="s">
-        <v>91</v>
-      </c>
-      <c r="P34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P34">
+        <v>0.2</v>
+      </c>
+      <c r="S34">
+        <v>0.2</v>
+      </c>
+      <c r="T34">
+        <v>-0.25</v>
+      </c>
+      <c r="U34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2265,14 +2351,17 @@
       <c r="N35">
         <v>0.2</v>
       </c>
-      <c r="O35" t="s">
-        <v>94</v>
-      </c>
-      <c r="P35" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P35">
+        <v>0.2</v>
+      </c>
+      <c r="T35">
+        <v>-0.25</v>
+      </c>
+      <c r="U35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2295,7 +2384,7 @@
         <v>30</v>
       </c>
       <c r="K36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -2306,14 +2395,23 @@
       <c r="N36">
         <v>0.2</v>
       </c>
-      <c r="O36" t="s">
-        <v>95</v>
-      </c>
-      <c r="P36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="P36">
+        <v>0.2</v>
+      </c>
+      <c r="Q36">
+        <v>-0.5</v>
+      </c>
+      <c r="S36">
+        <v>0.2</v>
+      </c>
+      <c r="T36">
+        <v>-0.25</v>
+      </c>
+      <c r="U36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2344,11 +2442,14 @@
       <c r="N37">
         <v>-0.15</v>
       </c>
-      <c r="O37" t="s">
-        <v>117</v>
-      </c>
-      <c r="P37" t="s">
-        <v>96</v>
+      <c r="P37">
+        <v>0.2</v>
+      </c>
+      <c r="T37">
+        <v>-0.25</v>
+      </c>
+      <c r="U37" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>